<commit_message>
Solve an issue on a keepout area.
</commit_message>
<xml_diff>
--- a/hardware/udriver3/uOmodri_v2_BOM.xlsx
+++ b/hardware/udriver3/uOmodri_v2_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmanhes\LAAS\Actionneur\github\open-motor-driver-initiative\hardware\udriver3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE0EB57A-E71D-4EBC-B97B-5A99CB0DE16D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD3670AB-23F7-410B-80E6-E4DF92038E69}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{F01C59C3-4777-4DE8-8383-5DB04A250DAD}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="354">
   <si>
     <t>10uF</t>
   </si>
@@ -795,39 +795,6 @@
     <t>Footprint</t>
   </si>
   <si>
-    <t>&gt;  C4-C6, C9-C11, C30, C32-C36, C43, C45-C49</t>
-  </si>
-  <si>
-    <t>&gt;  C29, C42</t>
-  </si>
-  <si>
-    <t>&gt;  C3, C7, C8, C12-C14, C19-C23, C26, C31, C39, C44, C50-C55, C69, C72-C94, C99-C104</t>
-  </si>
-  <si>
-    <t>&gt;  C1, C2</t>
-  </si>
-  <si>
-    <t>&gt;  C24, C27, C37, C40</t>
-  </si>
-  <si>
-    <t>&gt;  C28, C41, C61, C64, C67, C68, C71</t>
-  </si>
-  <si>
-    <t>&gt;  C25, C38</t>
-  </si>
-  <si>
-    <t>&gt;  C56, C57, C95, C96</t>
-  </si>
-  <si>
-    <t>&gt;  C60, C62, C63, C65, C66, C70</t>
-  </si>
-  <si>
-    <t>&gt;  C15-C18</t>
-  </si>
-  <si>
-    <t>&gt;  C59, C98</t>
-  </si>
-  <si>
     <t>Capacitor_SMD:C_0805_2012Metric</t>
   </si>
   <si>
@@ -843,21 +810,6 @@
     <t>247-8112</t>
   </si>
   <si>
-    <t>&gt;  R31, R32, R39-R41, R47</t>
-  </si>
-  <si>
-    <t>&gt;  R62, R64, R67, R68</t>
-  </si>
-  <si>
-    <t>&gt;  R18-R20</t>
-  </si>
-  <si>
-    <t>&gt;  R5, R6, R27, R30, R33-R35, R42-R44, R55, R56</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    R58</t>
-  </si>
-  <si>
     <t>P123194TR-ND</t>
   </si>
   <si>
@@ -867,48 +819,12 @@
     <t>ERJ-1GNF9090C</t>
   </si>
   <si>
-    <t>&gt;  R7-R12, R17, R37, R45</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    R50</t>
-  </si>
-  <si>
     <t>2.49k</t>
   </si>
   <si>
-    <t xml:space="preserve">    R25</t>
-  </si>
-  <si>
-    <t>&gt;  R1-R4, R14-R16, R21-R23, R26, R28, R29, R36, R38, R46, R48, R57, R59-R61, R65, R66</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    R52</t>
-  </si>
-  <si>
-    <t>&gt;  R13, R49, R51, R53, R54</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    R24</t>
-  </si>
-  <si>
-    <t>&gt;  FB1-FB3</t>
-  </si>
-  <si>
-    <t>&gt;  U1-U3, U19</t>
-  </si>
-  <si>
     <t>udriver3:SOT886_USON_6_1.45x1.0mm_P0.5mm</t>
   </si>
   <si>
-    <t>&gt;  J8, J9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    SW1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    D2</t>
-  </si>
-  <si>
     <t>BAT54L</t>
   </si>
   <si>
@@ -921,135 +837,30 @@
     <t>BAT54L,315</t>
   </si>
   <si>
-    <t xml:space="preserve">    U16</t>
-  </si>
-  <si>
     <t>BMI088</t>
   </si>
   <si>
     <t>udriver3:Bosch_LGA-16_4.5x3.0mm_P0.5mm</t>
   </si>
   <si>
-    <t xml:space="preserve">    J6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    J13</t>
-  </si>
-  <si>
-    <t>&gt;  J10, J11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    J1</t>
-  </si>
-  <si>
     <t>conn_01x04_MountingPins</t>
   </si>
   <si>
-    <t>&gt;  J2, J3, J14</t>
-  </si>
-  <si>
-    <t>&gt;  J4, J5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    J12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    J7</t>
-  </si>
-  <si>
-    <t>&gt;  Q2-Q7</t>
-  </si>
-  <si>
-    <t>&gt;  U9, U10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    U4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    U5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    X1</t>
-  </si>
-  <si>
-    <t>&gt;  D11, D12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    D6</t>
-  </si>
-  <si>
-    <t>&gt;  D9, D10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    U14</t>
-  </si>
-  <si>
-    <t>&gt;  H1-H4</t>
-  </si>
-  <si>
-    <t>MountingHole</t>
-  </si>
-  <si>
-    <t>MountingHole:MountingHole_2.2mm_M2</t>
-  </si>
-  <si>
-    <t>&gt;  U12, U13</t>
-  </si>
-  <si>
     <t>946-MPM3804GG-Z</t>
   </si>
   <si>
-    <t xml:space="preserve">    Q1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    U17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    U18</t>
-  </si>
-  <si>
     <t>THVD24x0</t>
   </si>
   <si>
-    <t xml:space="preserve">    U6</t>
-  </si>
-  <si>
-    <t>&gt;  D5, D7, D8</t>
-  </si>
-  <si>
-    <t>&gt;  D1, D3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    U8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    U7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    U15</t>
-  </si>
-  <si>
     <t>TPSM560R6H</t>
   </si>
   <si>
     <t>udriver3:B3QFN_15</t>
   </si>
   <si>
-    <t xml:space="preserve">    U11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    J15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    D4</t>
-  </si>
-  <si>
     <t>F28388DZWTS</t>
   </si>
   <si>
-    <t>v  C58, C97</t>
-  </si>
-  <si>
     <t>262-BMI088</t>
   </si>
   <si>
@@ -1075,13 +886,214 @@
   </si>
   <si>
     <t>595-TPSM560R6HRDAR</t>
+  </si>
+  <si>
+    <t>C4, C5, C6, C9, C10, C11, C30, C32, C33, C34, C35, C36, C43, C45, C46, C47, C48, C49</t>
+  </si>
+  <si>
+    <t>C29, C42</t>
+  </si>
+  <si>
+    <t>C3, C7, C8, C12, C13, C14, C19, C20, C21, C22, C23, C26, C31, C39, C44, C50, C51, C52, C53, C54, C55, C69, C72, C73, C74, C75, C76, C77, C78, C79, C80, C81, C82, C83, C84, C85, C86, C87, C88, C89, C90, C91, C92, C93, C94, C99, C100, C101, C102, C103, C104</t>
+  </si>
+  <si>
+    <t>C58, C97</t>
+  </si>
+  <si>
+    <t>C1, C2</t>
+  </si>
+  <si>
+    <t>C24, C27, C37, C40</t>
+  </si>
+  <si>
+    <t>C28, C41, C61, C64, C67, C68, C71</t>
+  </si>
+  <si>
+    <t>C25, C38</t>
+  </si>
+  <si>
+    <t>C56, C57, C95, C96</t>
+  </si>
+  <si>
+    <t>C60, C62, C63, C65, C66, C70</t>
+  </si>
+  <si>
+    <t>C15, C16, C17, C18</t>
+  </si>
+  <si>
+    <t>C59, C98</t>
+  </si>
+  <si>
+    <t>R31, R32, R39, R40, R41, R47</t>
+  </si>
+  <si>
+    <t>R62, R64, R67, R68</t>
+  </si>
+  <si>
+    <t>R18, R19, R20</t>
+  </si>
+  <si>
+    <t>R5, R6, R27, R30, R33, R34, R35, R42, R43, R44, R55, R56</t>
+  </si>
+  <si>
+    <t>R7, R8, R9, R10, R11, R12, R17, R37, R45</t>
+  </si>
+  <si>
+    <t>R1, R2, R3, R4, R14, R15, R16, R21, R22, R23, R26, R28, R29, R36, R38, R46, R48, R57, R59, R60, R61, R65, R66</t>
+  </si>
+  <si>
+    <t>R13, R49, R51, R53, R54</t>
+  </si>
+  <si>
+    <t>FB1, FB2, FB3</t>
+  </si>
+  <si>
+    <t>U1, U2, U3, U19</t>
+  </si>
+  <si>
+    <t>J8, J9</t>
+  </si>
+  <si>
+    <t>J10, J11</t>
+  </si>
+  <si>
+    <t>J2, J3, J14</t>
+  </si>
+  <si>
+    <t>J4, J5</t>
+  </si>
+  <si>
+    <t>Q2, Q3, Q4, Q5, Q6, Q7</t>
+  </si>
+  <si>
+    <t>U9, U10</t>
+  </si>
+  <si>
+    <t>D11, D12</t>
+  </si>
+  <si>
+    <t>D9, D10</t>
+  </si>
+  <si>
+    <t>U12, U13</t>
+  </si>
+  <si>
+    <t>D5, D7, D8</t>
+  </si>
+  <si>
+    <t>D1, D3</t>
+  </si>
+  <si>
+    <t>U8</t>
+  </si>
+  <si>
+    <t>U7</t>
+  </si>
+  <si>
+    <t>U15</t>
+  </si>
+  <si>
+    <t>U11</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> U6</t>
+  </si>
+  <si>
+    <t>U18</t>
+  </si>
+  <si>
+    <t>U17</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>U14</t>
+  </si>
+  <si>
+    <t>D6</t>
+  </si>
+  <si>
+    <t>X1</t>
+  </si>
+  <si>
+    <t>U5</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> U4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> J7</t>
+  </si>
+  <si>
+    <t>J12</t>
+  </si>
+  <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>J13</t>
+  </si>
+  <si>
+    <t>J6</t>
+  </si>
+  <si>
+    <t>U16</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>SW1</t>
+  </si>
+  <si>
+    <t>R24</t>
+  </si>
+  <si>
+    <t>R52</t>
+  </si>
+  <si>
+    <t>R25</t>
+  </si>
+  <si>
+    <t>R50</t>
+  </si>
+  <si>
+    <t>R58</t>
+  </si>
+  <si>
+    <t>J15</t>
+  </si>
+  <si>
+    <t>100+</t>
+  </si>
+  <si>
+    <t>150+</t>
+  </si>
+  <si>
+    <t>250+</t>
+  </si>
+  <si>
+    <t>200+</t>
+  </si>
+  <si>
+    <t>11+50(SMRTAT)</t>
+  </si>
+  <si>
+    <t>20 + 18(F28386)</t>
+  </si>
+  <si>
+    <t>130 + 50 (CSD88584)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1097,13 +1109,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -1130,18 +1166,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1150,9 +1185,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Neutre" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Satisfaisant" xfId="1" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1464,15 +1513,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C30724CF-18E3-4D71-A021-3C05174B3189}">
-  <dimension ref="A1:J62"/>
+  <dimension ref="A1:J61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F59" sqref="F59"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="50.5703125" style="2" customWidth="1"/>
     <col min="2" max="2" width="26.140625" style="2" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" style="2"/>
     <col min="4" max="4" width="46.85546875" style="2" customWidth="1"/>
@@ -1516,9 +1565,9 @@
         <v>225</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>256</v>
+        <v>287</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>19</v>
@@ -1542,11 +1591,13 @@
         <v>2999522</v>
       </c>
       <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-    </row>
-    <row r="3" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J2" s="5">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>257</v>
+        <v>288</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>34</v>
@@ -1570,11 +1621,13 @@
         <v>2906791</v>
       </c>
       <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-    </row>
-    <row r="4" spans="1:10" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="J3" s="5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>258</v>
+        <v>289</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>5</v>
@@ -1600,11 +1653,13 @@
       <c r="I4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="J4" s="5"/>
-    </row>
-    <row r="5" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J4" s="5">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>340</v>
+        <v>290</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>5</v>
@@ -1628,11 +1683,13 @@
         <v>1828921</v>
       </c>
       <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-    </row>
-    <row r="6" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J5" s="5" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>259</v>
+        <v>291</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>224</v>
@@ -1656,11 +1713,13 @@
         <v>3785715</v>
       </c>
       <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-    </row>
-    <row r="7" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J6" s="5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>260</v>
+        <v>292</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>27</v>
@@ -1684,11 +1743,13 @@
         <v>3416060</v>
       </c>
       <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-    </row>
-    <row r="8" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J7" s="5" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>261</v>
+        <v>293</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>27</v>
@@ -1712,11 +1773,13 @@
         <v>3238032</v>
       </c>
       <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-    </row>
-    <row r="9" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J8" s="5" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>262</v>
+        <v>294</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>0</v>
@@ -1742,11 +1805,13 @@
       <c r="I9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="J9" s="5"/>
-    </row>
-    <row r="10" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J9" s="5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>263</v>
+        <v>295</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>0</v>
@@ -1770,11 +1835,13 @@
         <v>3416259</v>
       </c>
       <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-    </row>
-    <row r="11" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J10" s="5" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>264</v>
+        <v>296</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>0</v>
@@ -1798,11 +1865,13 @@
         <v>3582794</v>
       </c>
       <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-    </row>
-    <row r="12" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J11" s="5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>265</v>
+        <v>297</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>38</v>
@@ -1826,41 +1895,43 @@
         <v>3416277</v>
       </c>
       <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-    </row>
-    <row r="13" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>266</v>
-      </c>
-      <c r="B13" s="5" t="s">
+      <c r="J12" s="5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="4">
         <v>2</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>270</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>267</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>269</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>268</v>
-      </c>
-      <c r="H13" s="5">
+      <c r="D13" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="H13" s="4">
         <v>1907510</v>
       </c>
-      <c r="I13" s="5" t="s">
-        <v>271</v>
-      </c>
-      <c r="J13" s="5"/>
-    </row>
-    <row r="14" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I13" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="J13" s="4"/>
+    </row>
+    <row r="14" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>272</v>
+        <v>299</v>
       </c>
       <c r="B14" s="5">
         <v>5.0000000000000001E-3</v>
@@ -1886,11 +1957,13 @@
       <c r="I14" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="J14" s="5"/>
-    </row>
-    <row r="15" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J14" s="5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>273</v>
+        <v>300</v>
       </c>
       <c r="B15" s="5">
         <v>10</v>
@@ -1916,11 +1989,13 @@
       <c r="I15" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="J15" s="5"/>
-    </row>
-    <row r="16" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J15" s="5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>274</v>
+        <v>301</v>
       </c>
       <c r="B16" s="5">
         <v>100</v>
@@ -1946,11 +2021,13 @@
       <c r="I16" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="J16" s="5"/>
-    </row>
-    <row r="17" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J16" s="5" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>275</v>
+        <v>302</v>
       </c>
       <c r="B17" s="5">
         <v>120</v>
@@ -1974,39 +2051,41 @@
         <v>2396857</v>
       </c>
       <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-    </row>
-    <row r="18" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="B18" s="5">
+      <c r="J17" s="5" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="B18" s="4">
         <v>909</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="4">
         <v>1</v>
       </c>
-      <c r="D18" s="5" t="s">
-        <v>279</v>
-      </c>
-      <c r="E18" s="5" t="s">
+      <c r="D18" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="E18" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="F18" s="5" t="s">
-        <v>278</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="H18" s="5">
+      <c r="F18" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="H18" s="4">
         <v>3303125</v>
       </c>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-    </row>
-    <row r="19" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+    </row>
+    <row r="19" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>280</v>
+        <v>303</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>127</v>
@@ -2032,39 +2111,41 @@
       <c r="I19" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="J19" s="5"/>
-    </row>
-    <row r="20" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>281</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>282</v>
-      </c>
-      <c r="C20" s="5">
+      <c r="J19" s="5" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="C20" s="4">
         <v>1</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="E20" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="F20" s="5" t="s">
+      <c r="F20" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="G20" s="5" t="s">
+      <c r="G20" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="H20" s="5">
+      <c r="H20" s="4">
         <v>3335262</v>
       </c>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-    </row>
-    <row r="21" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+    </row>
+    <row r="21" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>283</v>
+        <v>343</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>146</v>
@@ -2090,41 +2171,45 @@
       <c r="I21" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="J21" s="5"/>
-    </row>
-    <row r="22" spans="1:10" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
-        <v>284</v>
-      </c>
-      <c r="B22" s="5" t="s">
+      <c r="J21" s="5" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>304</v>
+      </c>
+      <c r="B22" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C22" s="6">
         <v>23</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="E22" s="5" t="s">
+      <c r="E22" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="F22" s="5" t="s">
+      <c r="F22" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="G22" s="5" t="s">
+      <c r="G22" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="H22" s="5">
+      <c r="H22" s="6">
         <v>2302362</v>
       </c>
-      <c r="I22" s="5" t="s">
+      <c r="I22" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="J22" s="5"/>
-    </row>
-    <row r="23" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J22" s="6" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>285</v>
+        <v>342</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>123</v>
@@ -2148,11 +2233,13 @@
         <v>3335196</v>
       </c>
       <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
-    </row>
-    <row r="24" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J23" s="5" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>286</v>
+        <v>305</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>118</v>
@@ -2178,11 +2265,13 @@
       <c r="I24" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="J24" s="5"/>
-    </row>
-    <row r="25" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J24" s="5" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>287</v>
+        <v>341</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>118</v>
@@ -2208,11 +2297,13 @@
       <c r="I25" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="J25" s="5"/>
-    </row>
-    <row r="26" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J25" s="5" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>288</v>
+        <v>306</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>67</v>
@@ -2238,11 +2329,13 @@
       <c r="I26" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="J26" s="5"/>
-    </row>
-    <row r="27" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J26" s="5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>289</v>
+        <v>307</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>177</v>
@@ -2254,7 +2347,7 @@
         <v>254</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>290</v>
+        <v>265</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>253</v>
@@ -2264,41 +2357,43 @@
       </c>
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
-      <c r="J27" s="5"/>
-    </row>
-    <row r="28" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
-        <v>291</v>
-      </c>
-      <c r="B28" s="5" t="s">
+      <c r="J27" s="5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="B28" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C28" s="5">
+      <c r="C28" s="4">
         <v>2</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D28" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="E28" s="5" t="s">
+      <c r="E28" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="F28" s="5" t="s">
+      <c r="F28" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="G28" s="5" t="s">
+      <c r="G28" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="H28" s="5">
+      <c r="H28" s="4">
         <v>3462763</v>
       </c>
-      <c r="I28" s="5" t="s">
+      <c r="I28" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="J28" s="5"/>
-    </row>
-    <row r="29" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J28" s="4"/>
+    </row>
+    <row r="29" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>292</v>
+        <v>340</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>160</v>
@@ -2322,84 +2417,89 @@
         <v>1333654</v>
       </c>
       <c r="I29" s="5"/>
-      <c r="J29" s="5"/>
-    </row>
-    <row r="30" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
-        <v>293</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>294</v>
-      </c>
-      <c r="C30" s="5">
+      <c r="J29" s="5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="C30" s="4">
         <v>1</v>
       </c>
-      <c r="D30" s="5" t="s">
-        <v>297</v>
-      </c>
-      <c r="E30" s="5" t="s">
+      <c r="D30" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="E30" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="F30" s="5" t="s">
-        <v>296</v>
-      </c>
-      <c r="G30" s="5" t="s">
-        <v>295</v>
-      </c>
-      <c r="H30" s="5">
+      <c r="F30" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="H30" s="4">
         <v>2438976</v>
       </c>
-      <c r="I30" s="5"/>
-      <c r="J30" s="5"/>
-    </row>
-    <row r="31" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
-        <v>298</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>299</v>
-      </c>
-      <c r="C31" s="5">
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
+    </row>
+    <row r="31" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>338</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="C31" s="6">
         <v>1</v>
       </c>
-      <c r="D31" s="5" t="s">
-        <v>299</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>300</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>341</v>
-      </c>
-      <c r="G31" s="5" t="s">
-        <v>342</v>
-      </c>
-      <c r="I31" s="5"/>
-      <c r="J31" s="5"/>
-    </row>
-    <row r="32" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
-        <v>301</v>
-      </c>
-      <c r="B32" s="5" t="s">
+      <c r="D31" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="H31" s="7"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="B32" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C32" s="5">
+      <c r="C32" s="4">
         <v>1</v>
       </c>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5" t="s">
+      <c r="D32" s="4"/>
+      <c r="E32" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
-      <c r="H32" s="5"/>
-      <c r="I32" s="5"/>
-      <c r="J32" s="5"/>
-    </row>
-    <row r="33" spans="1:10" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="4"/>
+    </row>
+    <row r="33" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>302</v>
+        <v>336</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>76</v>
@@ -2423,34 +2523,36 @@
       <c r="I33" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="J33" s="5"/>
-    </row>
-    <row r="34" spans="1:10" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
-        <v>303</v>
-      </c>
-      <c r="B34" s="5" t="s">
+      <c r="J33" s="5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="B34" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C34" s="5">
+      <c r="C34" s="4">
         <v>2</v>
       </c>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5" t="s">
+      <c r="D34" s="4"/>
+      <c r="E34" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="F34" s="5"/>
-      <c r="G34" s="5"/>
-      <c r="H34" s="5"/>
-      <c r="I34" s="5"/>
-      <c r="J34" s="5"/>
-    </row>
-    <row r="35" spans="1:10" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="4"/>
+    </row>
+    <row r="35" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>304</v>
+        <v>335</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>305</v>
+        <v>272</v>
       </c>
       <c r="C35" s="5">
         <v>1</v>
@@ -2473,11 +2575,13 @@
       <c r="I35" s="5" t="s">
         <v>233</v>
       </c>
-      <c r="J35" s="5"/>
-    </row>
-    <row r="36" spans="1:10" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="J35" s="5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>73</v>
@@ -2503,11 +2607,13 @@
       <c r="I36" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="J36" s="5"/>
-    </row>
-    <row r="37" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J36" s="5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>85</v>
@@ -2533,39 +2639,43 @@
       <c r="I37" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="J37" s="5"/>
-    </row>
-    <row r="38" spans="1:10" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="5" t="s">
-        <v>308</v>
-      </c>
-      <c r="B38" s="5" t="s">
+      <c r="J37" s="5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="6" t="s">
+        <v>334</v>
+      </c>
+      <c r="B38" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="C38" s="5">
+      <c r="C38" s="6">
         <v>1</v>
       </c>
-      <c r="D38" s="5" t="s">
+      <c r="D38" s="6" t="s">
         <v>245</v>
       </c>
-      <c r="E38" s="5" t="s">
+      <c r="E38" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="F38" s="5" t="s">
+      <c r="F38" s="6" t="s">
         <v>238</v>
       </c>
-      <c r="G38" s="5" t="s">
+      <c r="G38" s="6" t="s">
         <v>235</v>
       </c>
-      <c r="H38" s="5"/>
-      <c r="I38" s="5" t="s">
+      <c r="H38" s="6"/>
+      <c r="I38" s="6" t="s">
         <v>241</v>
       </c>
-      <c r="J38" s="5"/>
-    </row>
-    <row r="39" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J38" s="6">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>309</v>
+        <v>333</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>80</v>
@@ -2589,11 +2699,13 @@
         <v>2892503</v>
       </c>
       <c r="I39" s="5"/>
-      <c r="J39" s="5"/>
-    </row>
-    <row r="40" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J39" s="5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>105</v>
@@ -2617,11 +2729,13 @@
         <v>2766880</v>
       </c>
       <c r="I40" s="5"/>
-      <c r="J40" s="5"/>
-    </row>
-    <row r="41" spans="1:10" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="J40" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>206</v>
@@ -2643,11 +2757,13 @@
       </c>
       <c r="H41" s="5"/>
       <c r="I41" s="5"/>
-      <c r="J41" s="5"/>
-    </row>
-    <row r="42" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J41" s="5" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>312</v>
+        <v>332</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>201</v>
@@ -2669,11 +2785,13 @@
       </c>
       <c r="H42" s="5"/>
       <c r="I42" s="5"/>
-      <c r="J42" s="5"/>
-    </row>
-    <row r="43" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J42" s="5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>313</v>
+        <v>331</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>182</v>
@@ -2695,11 +2813,13 @@
       </c>
       <c r="H43" s="5"/>
       <c r="I43" s="5"/>
-      <c r="J43" s="5"/>
-    </row>
-    <row r="44" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J43" s="5">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>314</v>
+        <v>330</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>211</v>
@@ -2723,11 +2843,13 @@
         <v>4059413</v>
       </c>
       <c r="I44" s="5"/>
-      <c r="J44" s="5"/>
-    </row>
-    <row r="45" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J44" s="5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B45" s="5" t="s">
         <v>62</v>
@@ -2749,11 +2871,13 @@
       </c>
       <c r="H45" s="5"/>
       <c r="I45" s="5"/>
-      <c r="J45" s="5"/>
-    </row>
-    <row r="46" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J45" s="5" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>316</v>
+        <v>329</v>
       </c>
       <c r="B46" s="5" t="s">
         <v>43</v>
@@ -2779,11 +2903,13 @@
       <c r="I46" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="J46" s="5"/>
-    </row>
-    <row r="47" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J46" s="5">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>49</v>
@@ -2807,11 +2933,13 @@
         <v>2494321</v>
       </c>
       <c r="I47" s="5"/>
-      <c r="J47" s="5"/>
-    </row>
-    <row r="48" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J47" s="5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>318</v>
+        <v>328</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>172</v>
@@ -2835,375 +2963,383 @@
         <v>2761957</v>
       </c>
       <c r="I48" s="5"/>
-      <c r="J48" s="5"/>
-    </row>
-    <row r="49" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J48" s="5">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="C49" s="5">
+        <v>2</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="G49" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="H49" s="5">
+        <v>3358188</v>
+      </c>
+      <c r="I49" s="5"/>
+      <c r="J49" s="5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="5" t="s">
+        <v>327</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C50" s="5">
+        <v>1</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G50" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="H50" s="5">
+        <v>2498574</v>
+      </c>
+      <c r="I50" s="5"/>
+      <c r="J50" s="5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="C51" s="8">
+        <v>1</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="G51" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="H51" s="5">
+        <v>3009407</v>
+      </c>
+      <c r="I51" s="5"/>
+      <c r="J51" s="5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A52" s="8" t="s">
+        <v>325</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>274</v>
+      </c>
+      <c r="C52" s="8">
+        <v>1</v>
+      </c>
+      <c r="D52" s="8" t="s">
+        <v>248</v>
+      </c>
+      <c r="E52" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="F52" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="G52" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="H52" s="8"/>
+      <c r="I52" s="8"/>
+      <c r="J52" s="8">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A53" s="8" t="s">
+        <v>324</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="C53" s="8">
+        <v>1</v>
+      </c>
+      <c r="D53" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="E53" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="F53" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="G53" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="H53" s="8"/>
+      <c r="I53" s="8"/>
+      <c r="J53" s="8" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" s="8" t="s">
+        <v>317</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C54" s="8">
+        <v>3</v>
+      </c>
+      <c r="D54" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="E54" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="F54" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="G54" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="H54" s="8"/>
+      <c r="I54" s="8"/>
+      <c r="J54" s="8">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" s="8" t="s">
+        <v>318</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="C55" s="8">
+        <v>2</v>
+      </c>
+      <c r="D55" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="E55" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="F55" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="G55" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="H55" s="8"/>
+      <c r="I55" s="8"/>
+      <c r="J55" s="8">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" s="8" t="s">
         <v>319</v>
       </c>
-      <c r="B49" s="5" t="s">
+      <c r="B56" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="C56" s="8">
+        <v>1</v>
+      </c>
+      <c r="D56" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="E56" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="F56" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="G56" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="H56" s="8"/>
+      <c r="I56" s="8"/>
+      <c r="J56" s="8">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" s="8" t="s">
         <v>320</v>
       </c>
-      <c r="C49" s="5">
-        <v>4</v>
-      </c>
-      <c r="D49" s="5"/>
-      <c r="E49" s="5" t="s">
+      <c r="B57" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="C57" s="8">
+        <v>1</v>
+      </c>
+      <c r="D57" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="E57" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="F57" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="G57" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="H57" s="8"/>
+      <c r="I57" s="8"/>
+      <c r="J57" s="8">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58" s="8" t="s">
         <v>321</v>
       </c>
-      <c r="F49" s="5"/>
-      <c r="G49" s="5"/>
-      <c r="H49" s="5"/>
-      <c r="I49" s="5"/>
-      <c r="J49" s="5"/>
-    </row>
-    <row r="50" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="5" t="s">
+      <c r="B58" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="C58" s="8">
+        <v>1</v>
+      </c>
+      <c r="D58" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="E58" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="F58" s="8" t="s">
+        <v>286</v>
+      </c>
+      <c r="G58" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="H58" s="8"/>
+      <c r="I58" s="8"/>
+      <c r="J58" s="8">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" s="8" t="s">
         <v>322</v>
       </c>
-      <c r="B50" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="C50" s="5">
-        <v>2</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="E50" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="F50" s="5" t="s">
+      <c r="B59" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="C59" s="8">
+        <v>1</v>
+      </c>
+      <c r="D59" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="E59" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="F59" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="G59" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="H59" s="8"/>
+      <c r="I59" s="8"/>
+      <c r="J59" s="8">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60" s="8" t="s">
+        <v>346</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C60" s="8">
+        <v>1</v>
+      </c>
+      <c r="D60" s="8">
+        <v>473460001</v>
+      </c>
+      <c r="E60" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="F60" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="G60" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="H60" s="8">
+        <v>1568026</v>
+      </c>
+      <c r="I60" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="J60" s="8">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61" s="8" t="s">
         <v>323</v>
       </c>
-      <c r="G50" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="H50" s="5">
-        <v>3358188</v>
-      </c>
-      <c r="I50" s="5"/>
-      <c r="J50" s="5"/>
-    </row>
-    <row r="51" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="5" t="s">
-        <v>324</v>
-      </c>
-      <c r="B51" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C51" s="5">
+      <c r="B61" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C61" s="8">
         <v>1</v>
       </c>
-      <c r="D51" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="E51" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="F51" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="G51" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="H51" s="5">
-        <v>2498574</v>
-      </c>
-      <c r="I51" s="5"/>
-      <c r="J51" s="5"/>
-    </row>
-    <row r="52" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="3" t="s">
-        <v>325</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="C52" s="3">
-        <v>1</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="E52" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="F52" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="G52" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="H52" s="5">
-        <v>3009407</v>
-      </c>
-      <c r="I52" s="5"/>
-      <c r="J52" s="5"/>
-    </row>
-    <row r="53" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A53" s="3" t="s">
-        <v>326</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>327</v>
-      </c>
-      <c r="C53" s="3">
-        <v>1</v>
-      </c>
-      <c r="D53" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="E53" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="F53" s="3" t="s">
-        <v>247</v>
-      </c>
-      <c r="G53" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="H53" s="3"/>
-      <c r="I53" s="3"/>
-      <c r="J53" s="3"/>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A54" s="3" t="s">
-        <v>328</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="C54" s="3">
-        <v>1</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>339</v>
-      </c>
-      <c r="E54" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="F54" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="G54" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="H54" s="3"/>
-      <c r="I54" s="3"/>
-      <c r="J54" s="3"/>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A55" s="3" t="s">
-        <v>329</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C55" s="3">
-        <v>3</v>
-      </c>
-      <c r="D55" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E55" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="F55" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G55" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="H55" s="3"/>
-      <c r="I55" s="3"/>
-      <c r="J55" s="3"/>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A56" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="C56" s="3">
-        <v>2</v>
-      </c>
-      <c r="D56" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="E56" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="F56" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="G56" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="H56" s="3"/>
-      <c r="I56" s="3"/>
-      <c r="J56" s="3"/>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A57" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="C57" s="3">
-        <v>1</v>
-      </c>
-      <c r="D57" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="E57" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="F57" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="G57" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="H57" s="3"/>
-      <c r="I57" s="3"/>
-      <c r="J57" s="3"/>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A58" s="3" t="s">
-        <v>332</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="C58" s="3">
-        <v>1</v>
-      </c>
-      <c r="D58" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="E58" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="F58" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="G58" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="H58" s="3"/>
-      <c r="I58" s="3"/>
-      <c r="J58" s="3"/>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A59" s="3" t="s">
-        <v>333</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="C59" s="3">
-        <v>1</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>344</v>
-      </c>
-      <c r="E59" s="3" t="s">
-        <v>335</v>
-      </c>
-      <c r="F59" s="3" t="s">
-        <v>349</v>
-      </c>
-      <c r="G59" s="3" t="s">
-        <v>347</v>
-      </c>
-      <c r="H59" s="3"/>
-      <c r="I59" s="3"/>
-      <c r="J59" s="3"/>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A60" s="3" t="s">
-        <v>336</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>343</v>
-      </c>
-      <c r="C60" s="3">
-        <v>1</v>
-      </c>
-      <c r="D60" s="3" t="s">
-        <v>345</v>
-      </c>
-      <c r="E60" s="3" t="s">
-        <v>335</v>
-      </c>
-      <c r="F60" s="3" t="s">
-        <v>348</v>
-      </c>
-      <c r="G60" s="3" t="s">
-        <v>346</v>
-      </c>
-      <c r="H60" s="3"/>
-      <c r="I60" s="3"/>
-      <c r="J60" s="3"/>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A61" s="3" t="s">
-        <v>337</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C61" s="3">
-        <v>1</v>
-      </c>
-      <c r="D61" s="3">
-        <v>473460001</v>
-      </c>
-      <c r="E61" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="F61" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="G61" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="H61" s="3">
-        <v>1568026</v>
-      </c>
-      <c r="I61" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="J61" s="3"/>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A62" s="3" t="s">
-        <v>338</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C62" s="3">
-        <v>1</v>
-      </c>
-      <c r="D62" s="3" t="s">
+      <c r="D61" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="E62" s="3" t="s">
+      <c r="E61" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="F62" s="3" t="s">
+      <c r="F61" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="G62" s="3" t="s">
+      <c r="G61" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="H62" s="3"/>
-      <c r="I62" s="3"/>
-      <c r="J62" s="3"/>
+      <c r="H61" s="8"/>
+      <c r="I61" s="8"/>
+      <c r="J61" s="8">
+        <v>50</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Issues solved on PCB to be build. - Drills too close to the edge board. - Mechanical pads of power transistor too close to edge board. - Some JTAG tracks didn't respect edge clearance.
</commit_message>
<xml_diff>
--- a/hardware/udriver3/uOmodri_v2_BOM.xlsx
+++ b/hardware/udriver3/uOmodri_v2_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmanhes\LAAS\Actionneur\github\open-motor-driver-initiative\hardware\udriver3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{017779D7-65EB-42FA-9BCB-FD537398EC5C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25651731-A3A0-4A91-BCEC-AE0F0A62696E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{F01C59C3-4777-4DE8-8383-5DB04A250DAD}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="357">
   <si>
     <t>10uF</t>
   </si>
@@ -1087,13 +1087,22 @@
   </si>
   <si>
     <t>P122865TR-ND</t>
+  </si>
+  <si>
+    <t>400+</t>
+  </si>
+  <si>
+    <t>5+10</t>
+  </si>
+  <si>
+    <t>11+10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1116,15 +1125,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1134,11 +1136,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -1166,12 +1163,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
@@ -1188,18 +1184,14 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Neutre" xfId="2" builtinId="28"/>
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Satisfaisant" xfId="1" builtinId="26"/>
   </cellStyles>
@@ -1516,7 +1508,7 @@
   <dimension ref="A1:J61"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1900,34 +1892,36 @@
       </c>
     </row>
     <row r="13" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="5" t="s">
         <v>295</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="5">
         <v>2</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="5" t="s">
         <v>256</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="F13" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="G13" s="5" t="s">
         <v>254</v>
       </c>
-      <c r="H13" s="4">
+      <c r="H13" s="5">
         <v>1907510</v>
       </c>
-      <c r="I13" s="4" t="s">
+      <c r="I13" s="5" t="s">
         <v>257</v>
       </c>
-      <c r="J13" s="4"/>
+      <c r="J13" s="5">
+        <v>50</v>
+      </c>
     </row>
     <row r="14" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
@@ -2056,32 +2050,34 @@
       </c>
     </row>
     <row r="18" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="5" t="s">
         <v>342</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18" s="5">
         <v>909</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="5">
         <v>1</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="5" t="s">
         <v>260</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E18" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="F18" s="5" t="s">
         <v>259</v>
       </c>
-      <c r="G18" s="4" t="s">
+      <c r="G18" s="5" t="s">
         <v>258</v>
       </c>
-      <c r="H18" s="4">
+      <c r="H18" s="5">
         <v>3303125</v>
       </c>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5">
+        <v>100</v>
+      </c>
     </row>
     <row r="19" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
@@ -2116,32 +2112,34 @@
       </c>
     </row>
     <row r="20" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="5" t="s">
         <v>341</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="5" t="s">
         <v>261</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20" s="5">
         <v>1</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="5" t="s">
         <v>351</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="E20" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="F20" s="4" t="s">
+      <c r="F20" s="5" t="s">
         <v>352</v>
       </c>
-      <c r="G20" s="4" t="s">
+      <c r="G20" s="5" t="s">
         <v>353</v>
       </c>
-      <c r="H20" s="4">
+      <c r="H20" s="5">
         <v>3335222</v>
       </c>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5">
+        <v>100</v>
+      </c>
     </row>
     <row r="21" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
@@ -2176,35 +2174,35 @@
       </c>
     </row>
     <row r="22" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="5" t="s">
         <v>301</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="C22" s="6">
+      <c r="C22" s="5">
         <v>23</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D22" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="E22" s="6" t="s">
+      <c r="E22" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="F22" s="6" t="s">
+      <c r="F22" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="G22" s="6" t="s">
+      <c r="G22" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="H22" s="6">
+      <c r="H22" s="5">
         <v>2302362</v>
       </c>
-      <c r="I22" s="6" t="s">
+      <c r="I22" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="J22" s="6" t="s">
-        <v>347</v>
+      <c r="J22" s="5" t="s">
+        <v>354</v>
       </c>
     </row>
     <row r="23" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -2422,59 +2420,61 @@
       </c>
     </row>
     <row r="30" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="5" t="s">
         <v>336</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="C30" s="4">
+      <c r="C30" s="5">
         <v>1</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D30" s="5" t="s">
         <v>266</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="E30" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="F30" s="4" t="s">
+      <c r="F30" s="5" t="s">
         <v>265</v>
       </c>
-      <c r="G30" s="4" t="s">
+      <c r="G30" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="H30" s="4">
+      <c r="H30" s="5">
         <v>2438976</v>
       </c>
-      <c r="I30" s="4"/>
-      <c r="J30" s="4"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5">
+        <v>25</v>
+      </c>
     </row>
     <row r="31" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
+      <c r="A31" s="5" t="s">
         <v>335</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="5" t="s">
         <v>267</v>
       </c>
-      <c r="C31" s="6">
+      <c r="C31" s="5">
         <v>1</v>
       </c>
-      <c r="D31" s="6" t="s">
+      <c r="D31" s="5" t="s">
         <v>267</v>
       </c>
-      <c r="E31" s="6" t="s">
+      <c r="E31" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="F31" s="6" t="s">
+      <c r="F31" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="G31" s="6" t="s">
+      <c r="G31" s="5" t="s">
         <v>276</v>
       </c>
       <c r="H31" s="7"/>
-      <c r="I31" s="6"/>
-      <c r="J31" s="6">
-        <v>5</v>
+      <c r="I31" s="5"/>
+      <c r="J31" s="5" t="s">
+        <v>355</v>
       </c>
     </row>
     <row r="32" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -2644,33 +2644,33 @@
       </c>
     </row>
     <row r="38" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="6" t="s">
+      <c r="A38" s="5" t="s">
         <v>331</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="B38" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C38" s="6">
+      <c r="C38" s="5">
         <v>1</v>
       </c>
-      <c r="D38" s="6" t="s">
+      <c r="D38" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="E38" s="6" t="s">
+      <c r="E38" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="F38" s="6" t="s">
+      <c r="F38" s="5" t="s">
         <v>238</v>
       </c>
-      <c r="G38" s="6" t="s">
+      <c r="G38" s="5" t="s">
         <v>235</v>
       </c>
-      <c r="H38" s="6"/>
-      <c r="I38" s="6" t="s">
+      <c r="H38" s="5"/>
+      <c r="I38" s="5" t="s">
         <v>241</v>
       </c>
-      <c r="J38" s="6">
-        <v>11</v>
+      <c r="J38" s="5" t="s">
+        <v>356</v>
       </c>
     </row>
     <row r="39" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -3028,13 +3028,13 @@
       </c>
     </row>
     <row r="51" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="8" t="s">
+      <c r="A51" s="6" t="s">
         <v>323</v>
       </c>
-      <c r="B51" s="8" t="s">
+      <c r="B51" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="C51" s="8">
+      <c r="C51" s="6">
         <v>1</v>
       </c>
       <c r="D51" s="5" t="s">
@@ -3058,286 +3058,286 @@
       </c>
     </row>
     <row r="52" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A52" s="8" t="s">
+      <c r="A52" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="B52" s="8" t="s">
+      <c r="B52" s="6" t="s">
         <v>271</v>
       </c>
-      <c r="C52" s="8">
+      <c r="C52" s="6">
         <v>1</v>
       </c>
-      <c r="D52" s="8" t="s">
+      <c r="D52" s="6" t="s">
         <v>245</v>
       </c>
-      <c r="E52" s="8" t="s">
+      <c r="E52" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="F52" s="8" t="s">
+      <c r="F52" s="6" t="s">
         <v>244</v>
       </c>
-      <c r="G52" s="8" t="s">
+      <c r="G52" s="6" t="s">
         <v>243</v>
       </c>
-      <c r="H52" s="8"/>
-      <c r="I52" s="8"/>
-      <c r="J52" s="8">
+      <c r="H52" s="6"/>
+      <c r="I52" s="6"/>
+      <c r="J52" s="6">
         <v>50</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A53" s="8" t="s">
+      <c r="A53" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="B53" s="8" t="s">
+      <c r="B53" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="C53" s="8">
+      <c r="C53" s="6">
         <v>1</v>
       </c>
-      <c r="D53" s="8" t="s">
+      <c r="D53" s="6" t="s">
         <v>274</v>
       </c>
-      <c r="E53" s="8" t="s">
+      <c r="E53" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="F53" s="8" t="s">
+      <c r="F53" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="G53" s="8" t="s">
+      <c r="G53" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="H53" s="8"/>
-      <c r="I53" s="8"/>
-      <c r="J53" s="8" t="s">
+      <c r="H53" s="6"/>
+      <c r="I53" s="6"/>
+      <c r="J53" s="6" t="s">
         <v>349</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A54" s="8" t="s">
+      <c r="A54" s="6" t="s">
         <v>314</v>
       </c>
-      <c r="B54" s="8" t="s">
+      <c r="B54" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="C54" s="8">
+      <c r="C54" s="6">
         <v>3</v>
       </c>
-      <c r="D54" s="8" t="s">
+      <c r="D54" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E54" s="8" t="s">
+      <c r="E54" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="F54" s="8" t="s">
+      <c r="F54" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="G54" s="8" t="s">
+      <c r="G54" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="H54" s="8"/>
-      <c r="I54" s="8"/>
-      <c r="J54" s="8">
+      <c r="H54" s="6"/>
+      <c r="I54" s="6"/>
+      <c r="J54" s="6">
         <v>50</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A55" s="8" t="s">
+      <c r="A55" s="6" t="s">
         <v>315</v>
       </c>
-      <c r="B55" s="8" t="s">
+      <c r="B55" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="C55" s="8">
+      <c r="C55" s="6">
         <v>2</v>
       </c>
-      <c r="D55" s="8" t="s">
+      <c r="D55" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="E55" s="8" t="s">
+      <c r="E55" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="F55" s="8" t="s">
+      <c r="F55" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="G55" s="8" t="s">
+      <c r="G55" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="H55" s="8"/>
-      <c r="I55" s="8"/>
-      <c r="J55" s="8">
+      <c r="H55" s="6"/>
+      <c r="I55" s="6"/>
+      <c r="J55" s="6">
         <v>200</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A56" s="8" t="s">
+      <c r="A56" s="6" t="s">
         <v>316</v>
       </c>
-      <c r="B56" s="8" t="s">
+      <c r="B56" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="C56" s="8">
+      <c r="C56" s="6">
         <v>1</v>
       </c>
-      <c r="D56" s="8" t="s">
+      <c r="D56" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="E56" s="8" t="s">
+      <c r="E56" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="F56" s="8" t="s">
+      <c r="F56" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="G56" s="8" t="s">
+      <c r="G56" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="H56" s="8"/>
-      <c r="I56" s="8"/>
-      <c r="J56" s="8">
+      <c r="H56" s="6"/>
+      <c r="I56" s="6"/>
+      <c r="J56" s="6">
         <v>50</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A57" s="8" t="s">
+      <c r="A57" s="6" t="s">
         <v>317</v>
       </c>
-      <c r="B57" s="8" t="s">
+      <c r="B57" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="C57" s="8">
+      <c r="C57" s="6">
         <v>1</v>
       </c>
-      <c r="D57" s="8" t="s">
+      <c r="D57" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="E57" s="8" t="s">
+      <c r="E57" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="F57" s="8" t="s">
+      <c r="F57" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="G57" s="8" t="s">
+      <c r="G57" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="H57" s="8"/>
-      <c r="I57" s="8"/>
-      <c r="J57" s="8">
+      <c r="H57" s="6"/>
+      <c r="I57" s="6"/>
+      <c r="J57" s="6">
         <v>50</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A58" s="8" t="s">
+      <c r="A58" s="6" t="s">
         <v>318</v>
       </c>
-      <c r="B58" s="8" t="s">
+      <c r="B58" s="6" t="s">
         <v>272</v>
       </c>
-      <c r="C58" s="8">
+      <c r="C58" s="6">
         <v>1</v>
       </c>
-      <c r="D58" s="8" t="s">
+      <c r="D58" s="6" t="s">
         <v>278</v>
       </c>
-      <c r="E58" s="8" t="s">
+      <c r="E58" s="6" t="s">
         <v>273</v>
       </c>
-      <c r="F58" s="8" t="s">
+      <c r="F58" s="6" t="s">
         <v>283</v>
       </c>
-      <c r="G58" s="8" t="s">
+      <c r="G58" s="6" t="s">
         <v>281</v>
       </c>
-      <c r="H58" s="8"/>
-      <c r="I58" s="8"/>
-      <c r="J58" s="8">
+      <c r="H58" s="6"/>
+      <c r="I58" s="6"/>
+      <c r="J58" s="6">
         <v>50</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A59" s="8" t="s">
+      <c r="A59" s="6" t="s">
         <v>319</v>
       </c>
-      <c r="B59" s="8" t="s">
+      <c r="B59" s="6" t="s">
         <v>277</v>
       </c>
-      <c r="C59" s="8">
+      <c r="C59" s="6">
         <v>1</v>
       </c>
-      <c r="D59" s="8" t="s">
+      <c r="D59" s="6" t="s">
         <v>279</v>
       </c>
-      <c r="E59" s="8" t="s">
+      <c r="E59" s="6" t="s">
         <v>273</v>
       </c>
-      <c r="F59" s="8" t="s">
+      <c r="F59" s="6" t="s">
         <v>282</v>
       </c>
-      <c r="G59" s="8" t="s">
+      <c r="G59" s="6" t="s">
         <v>280</v>
       </c>
-      <c r="H59" s="8"/>
-      <c r="I59" s="8"/>
-      <c r="J59" s="8">
+      <c r="H59" s="6"/>
+      <c r="I59" s="6"/>
+      <c r="J59" s="6">
         <v>50</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A60" s="8" t="s">
+      <c r="A60" s="6" t="s">
         <v>343</v>
       </c>
-      <c r="B60" s="8" t="s">
+      <c r="B60" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="C60" s="8">
+      <c r="C60" s="6">
         <v>1</v>
       </c>
-      <c r="D60" s="8">
+      <c r="D60" s="6">
         <v>473460001</v>
       </c>
-      <c r="E60" s="8" t="s">
+      <c r="E60" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F60" s="8" t="s">
+      <c r="F60" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="G60" s="8" t="s">
+      <c r="G60" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="H60" s="8">
+      <c r="H60" s="6">
         <v>1568026</v>
       </c>
-      <c r="I60" s="8" t="s">
+      <c r="I60" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="J60" s="8">
+      <c r="J60" s="6">
         <v>30</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A61" s="8" t="s">
+      <c r="A61" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="B61" s="8" t="s">
+      <c r="B61" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="C61" s="8">
+      <c r="C61" s="6">
         <v>1</v>
       </c>
-      <c r="D61" s="8" t="s">
+      <c r="D61" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="E61" s="8" t="s">
+      <c r="E61" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="F61" s="8" t="s">
+      <c r="F61" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="G61" s="8" t="s">
+      <c r="G61" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="H61" s="8"/>
-      <c r="I61" s="8"/>
-      <c r="J61" s="8">
+      <c r="H61" s="6"/>
+      <c r="I61" s="6"/>
+      <c r="J61" s="6">
         <v>50</v>
       </c>
     </row>

</xml_diff>